<commit_message>
logic table updated till trivia module
</commit_message>
<xml_diff>
--- a/_docs/Logic.xlsx
+++ b/_docs/Logic.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="340">
   <si>
     <t>Name</t>
   </si>
@@ -54,30 +54,18 @@
     <t>?!</t>
   </si>
   <si>
-    <t xml:space="preserve"> (A-&gt;bool)-&gt;bool</t>
-  </si>
-  <si>
     <t>(A-&gt;bool)-&gt;bool</t>
   </si>
   <si>
     <t>~</t>
   </si>
   <si>
-    <t xml:space="preserve"> bool-&gt;bool</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t xml:space="preserve"> bool</t>
-  </si>
-  <si>
     <t>\/</t>
   </si>
   <si>
-    <t xml:space="preserve"> bool-&gt;bool-&gt;bool</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>Definition</t>
-  </si>
-  <si>
     <t>tactics</t>
   </si>
   <si>
@@ -114,9 +99,6 @@
     <t>@</t>
   </si>
   <si>
-    <t xml:space="preserve"> (A-&gt;bool)-&gt;A</t>
-  </si>
-  <si>
     <t>T_DEF</t>
   </si>
   <si>
@@ -280,9 +262,6 @@
   </si>
   <si>
     <t>|- !t1:A t2:B. (\x. t1) t2 = t1</t>
-  </si>
-  <si>
-    <t>KO</t>
   </si>
   <si>
     <t>|- !t1 t2 t3. t1 /\ t2 /\ t3 &lt;=&gt; (t1 /\ t2) /\ t3</t>
@@ -956,6 +935,136 @@
   </si>
   <si>
     <t>inductive_type_store</t>
+  </si>
+  <si>
+    <t>trivia</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>one_REP</t>
+  </si>
+  <si>
+    <t>bool-&gt;bool</t>
+  </si>
+  <si>
+    <t>(A-&gt;bool)-&gt;A</t>
+  </si>
+  <si>
+    <t>1-&gt;bool</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>A-&gt;A</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>(B-&gt;C)-&gt;(A-&gt;B)-&gt;A-&gt;C)</t>
+  </si>
+  <si>
+    <t>composition of funcs</t>
+  </si>
+  <si>
+    <t>identity func</t>
+  </si>
+  <si>
+    <t>o_DEF</t>
+  </si>
+  <si>
+    <t>|- (o) (f:B-&gt;C) g = \x:A. f(g(x))</t>
+  </si>
+  <si>
+    <t>I_DEF</t>
+  </si>
+  <si>
+    <t>|- I = \x:A. x"</t>
+  </si>
+  <si>
+    <t>o_THM</t>
+  </si>
+  <si>
+    <t>|- !f:B-&gt;C. !g:A-&gt;B. !x:A. (f o g) x = f(g(x))</t>
+  </si>
+  <si>
+    <t>o_ASSOC</t>
+  </si>
+  <si>
+    <t>|- !f:C-&gt;D. !g:B-&gt;C. !h:A-&gt;B. f o (g o h) = (f o g) o h</t>
+  </si>
+  <si>
+    <t>I_THM</t>
+  </si>
+  <si>
+    <t>|- !x:A. I x = x</t>
+  </si>
+  <si>
+    <t>I_O_ID</t>
+  </si>
+  <si>
+    <t>|- !f:A-&gt;B. (I o f = f) /\ (f o I = f)</t>
+  </si>
+  <si>
+    <t>EXISTS_ONE_REP</t>
+  </si>
+  <si>
+    <t>|- ?b:bool. B</t>
+  </si>
+  <si>
+    <t>one_ABS</t>
+  </si>
+  <si>
+    <t>one_tydef</t>
+  </si>
+  <si>
+    <t>|- (!a. one_ABS (one_REP a) = a) /\ (!r. r &lt;=&gt; one_REP (one_ABS r) &lt;=&gt; r)</t>
+  </si>
+  <si>
+    <t>bool-&gt;1</t>
+  </si>
+  <si>
+    <t>one_DEF</t>
+  </si>
+  <si>
+    <t>|- one = @x:1. T</t>
+  </si>
+  <si>
+    <t>|- !v:1. v = one</t>
+  </si>
+  <si>
+    <t>one_axiom</t>
+  </si>
+  <si>
+    <t>|- !f g. f = (g:A-&gt;1)</t>
+  </si>
+  <si>
+    <t>one_INDUCT</t>
+  </si>
+  <si>
+    <t>|- !P. P one ==&gt; !x. P x</t>
+  </si>
+  <si>
+    <t>one_RECURSION</t>
+  </si>
+  <si>
+    <t>|- !e:A. ?fn. fn one = e</t>
+  </si>
+  <si>
+    <t>Statement</t>
+  </si>
+  <si>
+    <t>one_Axiom</t>
+  </si>
+  <si>
+    <t>|- !e:A. ?!fn. fn one = e</t>
+  </si>
+  <si>
+    <t>The theory "1"
+What is this?</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1095,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -995,18 +1104,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1335,21 +1438,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1381,9 +1495,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1406,6 +1517,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1424,44 +1563,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1764,13 +1897,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M128"/>
+  <dimension ref="A1:M145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B115" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B129" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I136" sqref="I136"/>
+      <selection pane="bottomRight" activeCell="I151" sqref="I151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1779,62 +1912,62 @@
     <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="23" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="55.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" style="23" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>193</v>
-      </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="44"/>
+      <c r="B1" s="60" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="53"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="52"/>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="61"/>
+      <c r="B2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1848,28 +1981,28 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>25</v>
+        <v>336</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1937,7 +2070,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1945,13 +2078,13 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H7" s="8">
         <v>14</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="8"/>
@@ -1974,7 +2107,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="8"/>
@@ -1991,11 +2124,11 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="8"/>
@@ -2009,20 +2142,20 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8">
         <v>2</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="8"/>
@@ -2036,20 +2169,20 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
@@ -2061,10 +2194,10 @@
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2072,13 +2205,13 @@
         <v>8</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
@@ -2090,10 +2223,10 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2101,13 +2234,13 @@
         <v>4</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="L13" s="8"/>
       <c r="M13" s="9"/>
@@ -2119,7 +2252,7 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>12</v>
@@ -2128,13 +2261,13 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="9"/>
@@ -2146,7 +2279,7 @@
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>12</v>
@@ -2155,13 +2288,13 @@
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
@@ -2173,10 +2306,10 @@
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
@@ -2184,13 +2317,13 @@
         <v>6</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L16" s="8"/>
       <c r="M16" s="9"/>
@@ -2202,20 +2335,20 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="L17" s="8"/>
       <c r="M17" s="9"/>
@@ -2227,22 +2360,22 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>15</v>
+        <v>300</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="L18" s="8"/>
       <c r="M18" s="9"/>
@@ -2257,31 +2390,31 @@
         <v>11</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="L19" s="8"/>
       <c r="M19" s="9"/>
     </row>
     <row r="20" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>2</v>
@@ -2291,17 +2424,17 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L20" s="11"/>
       <c r="M20" s="9"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
@@ -2312,21 +2445,21 @@
       <c r="H21" s="8"/>
       <c r="I21" s="12"/>
       <c r="J21" s="13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="L21" s="38" t="s">
-        <v>194</v>
+        <v>68</v>
+      </c>
+      <c r="L21" s="47" t="s">
+        <v>187</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -2337,19 +2470,19 @@
       <c r="H22" s="8"/>
       <c r="I22" s="12"/>
       <c r="J22" s="16" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="L22" s="39"/>
+        <v>70</v>
+      </c>
+      <c r="L22" s="48"/>
       <c r="M22" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -2360,19 +2493,19 @@
       <c r="H23" s="8"/>
       <c r="I23" s="12"/>
       <c r="J23" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L23" s="39"/>
+        <v>73</v>
+      </c>
+      <c r="L23" s="48"/>
       <c r="M23" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2383,19 +2516,19 @@
       <c r="H24" s="8"/>
       <c r="I24" s="12"/>
       <c r="J24" s="16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="L24" s="39"/>
+        <v>74</v>
+      </c>
+      <c r="L24" s="48"/>
       <c r="M24" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2406,19 +2539,19 @@
       <c r="H25" s="8"/>
       <c r="I25" s="12"/>
       <c r="J25" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="L25" s="40"/>
+        <v>77</v>
+      </c>
+      <c r="L25" s="49"/>
       <c r="M25" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2429,19 +2562,19 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="19" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="L26" s="20"/>
       <c r="M26" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2452,19 +2585,19 @@
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
       <c r="J27" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L27" s="11"/>
-      <c r="M27" s="21" t="s">
-        <v>88</v>
+      <c r="M27" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2475,21 +2608,21 @@
       <c r="H28" s="8"/>
       <c r="I28" s="12"/>
       <c r="J28" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="L28" s="38" t="s">
-        <v>195</v>
+        <v>82</v>
+      </c>
+      <c r="L28" s="47" t="s">
+        <v>188</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2500,19 +2633,19 @@
       <c r="H29" s="8"/>
       <c r="I29" s="12"/>
       <c r="J29" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L29" s="39"/>
+        <v>84</v>
+      </c>
+      <c r="L29" s="48"/>
       <c r="M29" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2523,19 +2656,19 @@
       <c r="H30" s="8"/>
       <c r="I30" s="12"/>
       <c r="J30" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="K30" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="L30" s="39"/>
+        <v>86</v>
+      </c>
+      <c r="K30" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="L30" s="48"/>
       <c r="M30" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2546,21 +2679,21 @@
       <c r="H31" s="8"/>
       <c r="I31" s="12"/>
       <c r="J31" s="13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="L31" s="38" t="s">
-        <v>196</v>
+        <v>89</v>
+      </c>
+      <c r="L31" s="47" t="s">
+        <v>189</v>
       </c>
       <c r="M31" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2571,19 +2704,19 @@
       <c r="H32" s="8"/>
       <c r="I32" s="12"/>
       <c r="J32" s="16" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L32" s="39"/>
+        <v>90</v>
+      </c>
+      <c r="L32" s="48"/>
       <c r="M32" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2594,19 +2727,19 @@
       <c r="H33" s="8"/>
       <c r="I33" s="12"/>
       <c r="J33" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="K33" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="L33" s="39"/>
+        <v>92</v>
+      </c>
+      <c r="K33" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="L33" s="48"/>
       <c r="M33" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2617,21 +2750,21 @@
       <c r="H34" s="8"/>
       <c r="I34" s="12"/>
       <c r="J34" s="13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="L34" s="38" t="s">
-        <v>197</v>
+        <v>95</v>
+      </c>
+      <c r="L34" s="47" t="s">
+        <v>190</v>
       </c>
       <c r="M34" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2642,19 +2775,19 @@
       <c r="H35" s="8"/>
       <c r="I35" s="12"/>
       <c r="J35" s="16" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="L35" s="39"/>
+        <v>97</v>
+      </c>
+      <c r="L35" s="48"/>
       <c r="M35" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -2665,19 +2798,19 @@
       <c r="H36" s="8"/>
       <c r="I36" s="12"/>
       <c r="J36" s="17" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="K36" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="L36" s="40"/>
+        <v>99</v>
+      </c>
+      <c r="L36" s="49"/>
       <c r="M36" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -2688,19 +2821,19 @@
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="19" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="L37" s="20"/>
       <c r="M37" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -2711,19 +2844,19 @@
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="9" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="L38" s="8"/>
       <c r="M38" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2734,19 +2867,19 @@
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
       <c r="J39" s="9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="L39" s="8"/>
       <c r="M39" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2757,19 +2890,19 @@
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="L40" s="8"/>
       <c r="M40" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2780,19 +2913,19 @@
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
       <c r="J41" s="9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="L41" s="8"/>
       <c r="M41" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -2803,19 +2936,19 @@
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="L42" s="23"/>
+        <v>110</v>
+      </c>
+      <c r="K42" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="L42" s="22"/>
       <c r="M42" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -2826,19 +2959,19 @@
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
       <c r="J43" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="L43" s="8"/>
       <c r="M43" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -2849,19 +2982,19 @@
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="K44" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L44" s="23"/>
+        <v>114</v>
+      </c>
+      <c r="K44" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="L44" s="22"/>
       <c r="M44" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -2872,19 +3005,19 @@
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L45" s="23"/>
+        <v>116</v>
+      </c>
+      <c r="K45" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="L45" s="22"/>
       <c r="M45" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -2895,19 +3028,19 @@
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="K46" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L46" s="23"/>
+        <v>118</v>
+      </c>
+      <c r="K46" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="L46" s="22"/>
       <c r="M46" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -2918,19 +3051,19 @@
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
       <c r="J47" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="K47" s="8" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="L47" s="8"/>
-      <c r="M47" s="21" t="s">
-        <v>88</v>
+      <c r="M47" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -2941,19 +3074,19 @@
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K48" s="8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="L48" s="8"/>
       <c r="M48" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8"/>
@@ -2964,19 +3097,19 @@
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
       <c r="J49" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="L49" s="8"/>
-      <c r="M49" s="21" t="s">
-        <v>88</v>
+      <c r="M49" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
@@ -2987,19 +3120,19 @@
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="K50" s="8" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="L50" s="8"/>
       <c r="M50" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
@@ -3010,19 +3143,19 @@
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="9" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K51" s="8" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="L51" s="8"/>
       <c r="M51" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
@@ -3033,19 +3166,19 @@
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="K52" s="8" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L52" s="8"/>
       <c r="M52" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
@@ -3056,19 +3189,19 @@
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
       <c r="J53" s="9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="K53" s="8" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="L53" s="8"/>
       <c r="M53" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
@@ -3079,19 +3212,19 @@
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="9" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K54" s="8" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="L54" s="8"/>
       <c r="M54" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8"/>
@@ -3102,19 +3235,19 @@
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="L55" s="8"/>
       <c r="M55" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8"/>
@@ -3125,19 +3258,19 @@
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="K56" s="8" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="L56" s="8"/>
       <c r="M56" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -3148,19 +3281,19 @@
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
       <c r="J57" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="K57" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="L57" s="8"/>
       <c r="M57" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8"/>
@@ -3171,19 +3304,19 @@
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="9" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="K58" s="8" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="L58" s="8"/>
       <c r="M58" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
@@ -3194,19 +3327,19 @@
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
       <c r="J59" s="9" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="K59" s="8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="L59" s="8"/>
       <c r="M59" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8"/>
@@ -3217,19 +3350,19 @@
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="9" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="K60" s="8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="L60" s="8"/>
       <c r="M60" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
@@ -3240,19 +3373,19 @@
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
       <c r="J61" s="9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="K61" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="L61" s="8"/>
       <c r="M61" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8"/>
@@ -3263,19 +3396,19 @@
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="9" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K62" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="L62" s="8"/>
       <c r="M62" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B63" s="8"/>
       <c r="C63" s="8"/>
@@ -3286,19 +3419,19 @@
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
       <c r="J63" s="9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K63" s="8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="L63" s="8"/>
       <c r="M63" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="8"/>
@@ -3309,19 +3442,19 @@
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="9" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="K64" s="8" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="L64" s="8"/>
       <c r="M64" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="8"/>
@@ -3332,19 +3465,19 @@
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
       <c r="J65" s="9" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="K65" s="8" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="L65" s="8"/>
       <c r="M65" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="8"/>
@@ -3355,19 +3488,19 @@
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="9" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="L66" s="8"/>
       <c r="M66" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B67" s="8"/>
       <c r="C67" s="8"/>
@@ -3378,19 +3511,19 @@
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
       <c r="J67" s="9" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="K67" s="8" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="L67" s="8"/>
       <c r="M67" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3401,19 +3534,19 @@
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="9" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="K68" s="8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="L68" s="8"/>
       <c r="M68" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="8"/>
@@ -3424,19 +3557,19 @@
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
       <c r="J69" s="9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K69" s="8" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="L69" s="8"/>
       <c r="M69" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="8"/>
@@ -3447,19 +3580,19 @@
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="K70" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="L70" s="8"/>
       <c r="M70" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="8"/>
@@ -3470,19 +3603,19 @@
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
       <c r="J71" s="9" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="K71" s="8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="L71" s="8"/>
       <c r="M71" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="8"/>
@@ -3493,19 +3626,19 @@
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="9" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="L72" s="8"/>
       <c r="M72" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="8"/>
@@ -3516,19 +3649,19 @@
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
       <c r="J73" s="9" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L73" s="8"/>
       <c r="M73" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="8"/>
@@ -3539,19 +3672,19 @@
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="9" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K74" s="8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="L74" s="8"/>
       <c r="M74" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="8"/>
@@ -3562,19 +3695,19 @@
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="9" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K75" s="8" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="L75" s="8"/>
       <c r="M75" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="8"/>
@@ -3585,19 +3718,19 @@
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="9" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="K76" s="8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="L76" s="8"/>
       <c r="M76" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="8"/>
@@ -3608,19 +3741,19 @@
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
       <c r="J77" s="9" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="L77" s="8"/>
       <c r="M77" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="8"/>
@@ -3631,19 +3764,19 @@
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="9" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="L78" s="8"/>
-      <c r="M78" s="21" t="s">
-        <v>88</v>
+      <c r="M78" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="8"/>
@@ -3654,19 +3787,19 @@
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
       <c r="J79" s="10" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="K79" s="11" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="L79" s="11"/>
-      <c r="M79" s="21" t="s">
-        <v>88</v>
+      <c r="M79" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="8"/>
@@ -3677,21 +3810,21 @@
       <c r="H80" s="8"/>
       <c r="I80" s="12"/>
       <c r="J80" s="13" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="K80" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="L80" s="38" t="s">
-        <v>211</v>
+        <v>193</v>
+      </c>
+      <c r="L80" s="47" t="s">
+        <v>204</v>
       </c>
       <c r="M80" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="8"/>
@@ -3702,19 +3835,19 @@
       <c r="H81" s="8"/>
       <c r="I81" s="12"/>
       <c r="J81" s="16" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="L81" s="39"/>
+        <v>195</v>
+      </c>
+      <c r="L81" s="48"/>
       <c r="M81" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="8"/>
@@ -3725,19 +3858,19 @@
       <c r="H82" s="8"/>
       <c r="I82" s="12"/>
       <c r="J82" s="16" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="L82" s="39"/>
+        <v>197</v>
+      </c>
+      <c r="L82" s="48"/>
       <c r="M82" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="8"/>
@@ -3748,19 +3881,19 @@
       <c r="H83" s="8"/>
       <c r="I83" s="12"/>
       <c r="J83" s="16" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="L83" s="39"/>
+        <v>199</v>
+      </c>
+      <c r="L83" s="48"/>
       <c r="M83" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -3771,19 +3904,19 @@
       <c r="H84" s="8"/>
       <c r="I84" s="12"/>
       <c r="J84" s="16" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K84" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="L84" s="39"/>
+        <v>201</v>
+      </c>
+      <c r="L84" s="48"/>
       <c r="M84" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
@@ -3794,19 +3927,19 @@
       <c r="H85" s="8"/>
       <c r="I85" s="12"/>
       <c r="J85" s="17" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="K85" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="L85" s="40"/>
+        <v>203</v>
+      </c>
+      <c r="L85" s="49"/>
       <c r="M85" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -3817,88 +3950,88 @@
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="9" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K86" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="L86" s="8"/>
       <c r="M86" s="9"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B87" s="26"/>
-      <c r="C87" s="26"/>
-      <c r="D87" s="26"/>
-      <c r="E87" s="26"/>
-      <c r="F87" s="26"/>
-      <c r="G87" s="26"/>
-      <c r="H87" s="26"/>
-      <c r="I87" s="26"/>
-      <c r="J87" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="K87" s="26" t="s">
-        <v>213</v>
-      </c>
-      <c r="L87" s="26"/>
-      <c r="M87" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="25"/>
+      <c r="I87" s="25"/>
+      <c r="J87" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="K87" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="L87" s="25"/>
+      <c r="M87" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B88" s="26"/>
-      <c r="C88" s="26"/>
-      <c r="D88" s="26"/>
-      <c r="E88" s="26"/>
-      <c r="F88" s="26"/>
-      <c r="G88" s="26"/>
-      <c r="H88" s="26"/>
-      <c r="I88" s="26"/>
-      <c r="J88" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="K88" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="L88" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="M88" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+      <c r="I88" s="25"/>
+      <c r="J88" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="K88" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="L88" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="M88" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="72" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F89" s="25" t="s">
-        <v>219</v>
+        <v>301</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>212</v>
       </c>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
-      <c r="L89" s="26"/>
-      <c r="M89" s="26"/>
+      <c r="L89" s="25"/>
+      <c r="M89" s="25"/>
     </row>
     <row r="90" spans="1:13" ht="168" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -3909,923 +4042,1323 @@
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L90" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="M90" s="26"/>
+        <v>55</v>
+      </c>
+      <c r="L90" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="M90" s="25"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="26"/>
-      <c r="E91" s="26"/>
-      <c r="F91" s="26"/>
-      <c r="G91" s="26"/>
-      <c r="H91" s="26"/>
-      <c r="I91" s="26"/>
-      <c r="J91" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="K91" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="L91" s="26"/>
-      <c r="M91" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
+      <c r="F91" s="25"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="25"/>
+      <c r="I91" s="25"/>
+      <c r="J91" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="K91" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="L91" s="25"/>
+      <c r="M91" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="26"/>
-      <c r="E92" s="26"/>
-      <c r="F92" s="26"/>
-      <c r="G92" s="26"/>
-      <c r="H92" s="26"/>
-      <c r="I92" s="26"/>
-      <c r="J92" s="26" t="s">
-        <v>221</v>
-      </c>
-      <c r="K92" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="L92" s="26"/>
-      <c r="M92" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="25"/>
+      <c r="H92" s="25"/>
+      <c r="I92" s="25"/>
+      <c r="J92" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="K92" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="L92" s="25"/>
+      <c r="M92" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B93" s="26"/>
-      <c r="C93" s="26"/>
-      <c r="D93" s="26"/>
-      <c r="E93" s="26"/>
-      <c r="F93" s="26"/>
-      <c r="G93" s="26"/>
-      <c r="H93" s="26"/>
-      <c r="I93" s="26"/>
-      <c r="J93" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="K93" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="L93" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="M93" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="25"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
+      <c r="I93" s="25"/>
+      <c r="J93" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="K93" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="L93" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="M93" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="26"/>
-      <c r="E94" s="26"/>
-      <c r="F94" s="26"/>
-      <c r="G94" s="26"/>
-      <c r="H94" s="26"/>
-      <c r="I94" s="27"/>
-      <c r="J94" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="K94" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
+      <c r="F94" s="25"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="K94" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="L94" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="L94" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="M94" s="28" t="s">
-        <v>75</v>
+      <c r="M94" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="26"/>
-      <c r="E95" s="26"/>
-      <c r="F95" s="26"/>
-      <c r="G95" s="26"/>
-      <c r="H95" s="26"/>
-      <c r="I95" s="27"/>
-      <c r="J95" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="K95" s="26" t="s">
-        <v>229</v>
-      </c>
-      <c r="L95" s="39"/>
-      <c r="M95" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B95" s="25"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
+      <c r="F95" s="25"/>
+      <c r="G95" s="25"/>
+      <c r="H95" s="25"/>
+      <c r="I95" s="26"/>
+      <c r="J95" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="K95" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="L95" s="48"/>
+      <c r="M95" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B96" s="26"/>
-      <c r="C96" s="26"/>
-      <c r="D96" s="26"/>
-      <c r="E96" s="26"/>
-      <c r="F96" s="26"/>
-      <c r="G96" s="26"/>
-      <c r="H96" s="26"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="33" t="s">
-        <v>230</v>
-      </c>
-      <c r="K96" s="26" t="s">
-        <v>231</v>
-      </c>
-      <c r="L96" s="39"/>
-      <c r="M96" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B96" s="25"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
+      <c r="F96" s="25"/>
+      <c r="G96" s="25"/>
+      <c r="H96" s="25"/>
+      <c r="I96" s="26"/>
+      <c r="J96" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="K96" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="L96" s="48"/>
+      <c r="M96" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B97" s="26"/>
-      <c r="C97" s="26"/>
-      <c r="D97" s="26"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="26"/>
-      <c r="G97" s="26"/>
-      <c r="H97" s="26"/>
-      <c r="I97" s="27"/>
-      <c r="J97" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="K97" s="35" t="s">
-        <v>233</v>
-      </c>
-      <c r="L97" s="40"/>
-      <c r="M97" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B97" s="25"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
+      <c r="F97" s="25"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="25"/>
+      <c r="I97" s="26"/>
+      <c r="J97" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="K97" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="L97" s="49"/>
+      <c r="M97" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B98" s="26"/>
-      <c r="C98" s="26"/>
-      <c r="D98" s="26"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="26"/>
-      <c r="G98" s="26"/>
-      <c r="H98" s="26"/>
-      <c r="I98" s="27"/>
-      <c r="J98" s="31" t="s">
-        <v>235</v>
-      </c>
-      <c r="K98" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
+      <c r="F98" s="25"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="25"/>
+      <c r="I98" s="26"/>
+      <c r="J98" s="30" t="s">
+        <v>228</v>
+      </c>
+      <c r="K98" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="L98" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="L98" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="M98" s="28" t="s">
-        <v>75</v>
+      <c r="M98" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B99" s="26"/>
-      <c r="C99" s="26"/>
-      <c r="D99" s="26"/>
-      <c r="E99" s="26"/>
-      <c r="F99" s="26"/>
-      <c r="G99" s="26"/>
-      <c r="H99" s="26"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="K99" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="L99" s="41"/>
-      <c r="M99" s="21" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B99" s="25"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
+      <c r="F99" s="25"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="25"/>
+      <c r="I99" s="26"/>
+      <c r="J99" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="K99" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="L99" s="50"/>
+      <c r="M99" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B100" s="26"/>
-      <c r="C100" s="26"/>
-      <c r="D100" s="26"/>
-      <c r="E100" s="26"/>
-      <c r="F100" s="26"/>
-      <c r="G100" s="26"/>
-      <c r="H100" s="26"/>
-      <c r="I100" s="27"/>
-      <c r="J100" s="33" t="s">
-        <v>239</v>
-      </c>
-      <c r="K100" s="26" t="s">
-        <v>240</v>
-      </c>
-      <c r="L100" s="41"/>
-      <c r="M100" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
+      <c r="F100" s="25"/>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
+      <c r="I100" s="26"/>
+      <c r="J100" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="K100" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="L100" s="50"/>
+      <c r="M100" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B101" s="26"/>
-      <c r="C101" s="26"/>
-      <c r="D101" s="26"/>
-      <c r="E101" s="26"/>
-      <c r="F101" s="26"/>
-      <c r="G101" s="26"/>
-      <c r="H101" s="26"/>
-      <c r="I101" s="27"/>
-      <c r="J101" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="K101" s="35" t="s">
-        <v>242</v>
-      </c>
-      <c r="L101" s="37"/>
-      <c r="M101" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B101" s="25"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="25"/>
+      <c r="I101" s="26"/>
+      <c r="J101" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="K101" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="L101" s="46"/>
+      <c r="M101" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B102" s="26"/>
-      <c r="C102" s="26"/>
-      <c r="D102" s="26"/>
-      <c r="E102" s="26"/>
-      <c r="F102" s="26"/>
-      <c r="G102" s="26"/>
-      <c r="H102" s="26"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="K102" s="32" t="s">
-        <v>245</v>
-      </c>
-      <c r="L102" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="M102" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B102" s="25"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="25"/>
+      <c r="I102" s="26"/>
+      <c r="J102" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="K102" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="L102" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="M102" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B103" s="26"/>
-      <c r="C103" s="26"/>
-      <c r="D103" s="26"/>
-      <c r="E103" s="26"/>
-      <c r="F103" s="26"/>
-      <c r="G103" s="26"/>
-      <c r="H103" s="26"/>
-      <c r="I103" s="27"/>
-      <c r="J103" s="34" t="s">
-        <v>246</v>
-      </c>
-      <c r="K103" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="L103" s="37"/>
-      <c r="M103" s="21" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B103" s="25"/>
+      <c r="C103" s="25"/>
+      <c r="D103" s="25"/>
+      <c r="E103" s="25"/>
+      <c r="F103" s="25"/>
+      <c r="G103" s="25"/>
+      <c r="H103" s="25"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="K103" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="L103" s="46"/>
+      <c r="M103" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B104" s="26"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="26"/>
-      <c r="E104" s="26"/>
-      <c r="F104" s="26"/>
-      <c r="G104" s="26"/>
-      <c r="H104" s="26"/>
-      <c r="I104" s="27"/>
-      <c r="J104" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="K104" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="25"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
+      <c r="I104" s="26"/>
+      <c r="J104" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="K104" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="L104" s="47" t="s">
         <v>250</v>
       </c>
-      <c r="L104" s="38" t="s">
-        <v>257</v>
-      </c>
-      <c r="M104" s="53" t="s">
-        <v>88</v>
+      <c r="M104" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="26"/>
-      <c r="E105" s="26"/>
-      <c r="F105" s="26"/>
-      <c r="G105" s="26"/>
-      <c r="H105" s="26"/>
-      <c r="I105" s="27"/>
-      <c r="J105" s="33" t="s">
-        <v>251</v>
-      </c>
-      <c r="K105" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="L105" s="39"/>
-      <c r="M105" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B105" s="25"/>
+      <c r="C105" s="25"/>
+      <c r="D105" s="25"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="25"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="25"/>
+      <c r="I105" s="26"/>
+      <c r="J105" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="K105" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="L105" s="48"/>
+      <c r="M105" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B106" s="26"/>
-      <c r="C106" s="26"/>
-      <c r="D106" s="26"/>
-      <c r="E106" s="26"/>
-      <c r="F106" s="26"/>
-      <c r="G106" s="26"/>
-      <c r="H106" s="26"/>
-      <c r="I106" s="27"/>
-      <c r="J106" s="33" t="s">
-        <v>253</v>
-      </c>
-      <c r="K106" s="26" t="s">
-        <v>254</v>
-      </c>
-      <c r="L106" s="39"/>
-      <c r="M106" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B106" s="25"/>
+      <c r="C106" s="25"/>
+      <c r="D106" s="25"/>
+      <c r="E106" s="25"/>
+      <c r="F106" s="25"/>
+      <c r="G106" s="25"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="K106" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="L106" s="48"/>
+      <c r="M106" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A107" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B107" s="26"/>
-      <c r="C107" s="26"/>
-      <c r="D107" s="26"/>
-      <c r="E107" s="26"/>
-      <c r="F107" s="26"/>
-      <c r="G107" s="26"/>
-      <c r="H107" s="26"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="34" t="s">
-        <v>255</v>
-      </c>
-      <c r="K107" s="35" t="s">
-        <v>256</v>
-      </c>
-      <c r="L107" s="40"/>
-      <c r="M107" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B107" s="25"/>
+      <c r="C107" s="25"/>
+      <c r="D107" s="25"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="25"/>
+      <c r="G107" s="25"/>
+      <c r="H107" s="25"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="K107" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="L107" s="49"/>
+      <c r="M107" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" s="26"/>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
-      <c r="E108" s="26"/>
-      <c r="F108" s="26"/>
-      <c r="G108" s="26"/>
-      <c r="H108" s="26"/>
-      <c r="I108" s="27"/>
-      <c r="J108" s="31" t="s">
-        <v>258</v>
-      </c>
-      <c r="K108" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" s="25"/>
+      <c r="C108" s="25"/>
+      <c r="D108" s="25"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="25"/>
+      <c r="G108" s="25"/>
+      <c r="H108" s="25"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="K108" s="31" t="s">
+        <v>252</v>
+      </c>
+      <c r="L108" s="47" t="s">
         <v>259</v>
       </c>
-      <c r="L108" s="38" t="s">
-        <v>266</v>
-      </c>
-      <c r="M108" s="53" t="s">
-        <v>88</v>
+      <c r="M108" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B109" s="26"/>
-      <c r="C109" s="26"/>
-      <c r="D109" s="26"/>
-      <c r="E109" s="26"/>
-      <c r="F109" s="26"/>
-      <c r="G109" s="26"/>
-      <c r="H109" s="26"/>
-      <c r="I109" s="27"/>
-      <c r="J109" s="33" t="s">
-        <v>260</v>
-      </c>
-      <c r="K109" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="L109" s="39"/>
-      <c r="M109" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B109" s="25"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="25"/>
+      <c r="G109" s="25"/>
+      <c r="H109" s="25"/>
+      <c r="I109" s="26"/>
+      <c r="J109" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="K109" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="L109" s="48"/>
+      <c r="M109" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B110" s="26"/>
-      <c r="C110" s="26"/>
-      <c r="D110" s="26"/>
-      <c r="E110" s="26"/>
-      <c r="F110" s="26"/>
-      <c r="G110" s="26"/>
-      <c r="H110" s="26"/>
-      <c r="I110" s="27"/>
-      <c r="J110" s="33" t="s">
-        <v>262</v>
-      </c>
-      <c r="K110" s="26" t="s">
-        <v>263</v>
-      </c>
-      <c r="L110" s="39"/>
-      <c r="M110" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B110" s="25"/>
+      <c r="C110" s="25"/>
+      <c r="D110" s="25"/>
+      <c r="E110" s="25"/>
+      <c r="F110" s="25"/>
+      <c r="G110" s="25"/>
+      <c r="H110" s="25"/>
+      <c r="I110" s="26"/>
+      <c r="J110" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="K110" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="L110" s="48"/>
+      <c r="M110" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A111" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="26"/>
-      <c r="E111" s="26"/>
-      <c r="F111" s="26"/>
-      <c r="G111" s="26"/>
-      <c r="H111" s="26"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="K111" s="35" t="s">
-        <v>265</v>
-      </c>
-      <c r="L111" s="40"/>
-      <c r="M111" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B111" s="25"/>
+      <c r="C111" s="25"/>
+      <c r="D111" s="25"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="25"/>
+      <c r="H111" s="25"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="33" t="s">
+        <v>257</v>
+      </c>
+      <c r="K111" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="L111" s="49"/>
+      <c r="M111" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E112" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F112" s="26"/>
-      <c r="G112" s="26"/>
-      <c r="H112" s="26"/>
-      <c r="I112" s="26"/>
-      <c r="J112" s="29"/>
-      <c r="K112" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="L112" s="29"/>
-      <c r="M112" s="26"/>
+        <v>23</v>
+      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E112" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F112" s="25"/>
+      <c r="G112" s="25"/>
+      <c r="H112" s="25"/>
+      <c r="I112" s="25"/>
+      <c r="J112" s="28"/>
+      <c r="K112" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="L112" s="28"/>
+      <c r="M112" s="25"/>
     </row>
     <row r="113" spans="1:13" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B113" s="26"/>
-      <c r="C113" s="26"/>
-      <c r="D113" s="26"/>
-      <c r="E113" s="26"/>
-      <c r="F113" s="26"/>
-      <c r="G113" s="26"/>
-      <c r="H113" s="26"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="31" t="s">
-        <v>267</v>
-      </c>
-      <c r="K113" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="L113" s="38" t="s">
-        <v>279</v>
-      </c>
-      <c r="M113" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B113" s="25"/>
+      <c r="C113" s="25"/>
+      <c r="D113" s="25"/>
+      <c r="E113" s="25"/>
+      <c r="F113" s="25"/>
+      <c r="G113" s="25"/>
+      <c r="H113" s="25"/>
+      <c r="I113" s="26"/>
+      <c r="J113" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="K113" s="31" t="s">
+        <v>261</v>
+      </c>
+      <c r="L113" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="M113" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B114" s="26"/>
-      <c r="C114" s="26"/>
-      <c r="D114" s="26"/>
-      <c r="E114" s="26"/>
-      <c r="F114" s="26"/>
-      <c r="G114" s="26"/>
-      <c r="H114" s="26"/>
-      <c r="I114" s="27"/>
-      <c r="J114" s="33" t="s">
-        <v>269</v>
-      </c>
-      <c r="K114" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="L114" s="39"/>
-      <c r="M114" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B114" s="25"/>
+      <c r="C114" s="25"/>
+      <c r="D114" s="25"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="25"/>
+      <c r="G114" s="25"/>
+      <c r="H114" s="25"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="K114" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="L114" s="48"/>
+      <c r="M114" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B115" s="26"/>
-      <c r="C115" s="26"/>
-      <c r="D115" s="26"/>
-      <c r="E115" s="26"/>
-      <c r="F115" s="26"/>
-      <c r="G115" s="26"/>
-      <c r="H115" s="26"/>
-      <c r="I115" s="27"/>
-      <c r="J115" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="K115" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="L115" s="39"/>
-      <c r="M115" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B115" s="25"/>
+      <c r="C115" s="25"/>
+      <c r="D115" s="25"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="25"/>
+      <c r="G115" s="25"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="K115" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="L115" s="48"/>
+      <c r="M115" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="26"/>
-      <c r="E116" s="26"/>
-      <c r="F116" s="26"/>
-      <c r="G116" s="26"/>
-      <c r="H116" s="26"/>
-      <c r="I116" s="27"/>
-      <c r="J116" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="K116" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="L116" s="39"/>
-      <c r="M116" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B116" s="25"/>
+      <c r="C116" s="25"/>
+      <c r="D116" s="25"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="25"/>
+      <c r="G116" s="25"/>
+      <c r="H116" s="25"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="K116" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="L116" s="48"/>
+      <c r="M116" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B117" s="26"/>
-      <c r="C117" s="26"/>
-      <c r="D117" s="26"/>
-      <c r="E117" s="26"/>
-      <c r="F117" s="26"/>
-      <c r="G117" s="26"/>
-      <c r="H117" s="26"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="33" t="s">
-        <v>275</v>
-      </c>
-      <c r="K117" s="26" t="s">
-        <v>276</v>
-      </c>
-      <c r="L117" s="39"/>
-      <c r="M117" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B117" s="25"/>
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="25"/>
+      <c r="F117" s="25"/>
+      <c r="G117" s="25"/>
+      <c r="H117" s="25"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="K117" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="L117" s="48"/>
+      <c r="M117" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="118" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B118" s="26"/>
-      <c r="C118" s="26"/>
-      <c r="D118" s="26"/>
-      <c r="E118" s="26"/>
-      <c r="F118" s="26"/>
-      <c r="G118" s="26"/>
-      <c r="H118" s="26"/>
-      <c r="I118" s="27"/>
-      <c r="J118" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="K118" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="L118" s="39"/>
-      <c r="M118" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B118" s="25"/>
+      <c r="C118" s="25"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="25"/>
+      <c r="H118" s="25"/>
+      <c r="I118" s="26"/>
+      <c r="J118" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="K118" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="L118" s="48"/>
+      <c r="M118" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B119" s="26"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="26"/>
-      <c r="E119" s="26"/>
-      <c r="F119" s="26"/>
-      <c r="G119" s="26"/>
-      <c r="H119" s="26"/>
-      <c r="I119" s="27"/>
-      <c r="J119" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="K119" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="L119" s="39"/>
-      <c r="M119" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B119" s="25"/>
+      <c r="C119" s="25"/>
+      <c r="D119" s="25"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="25"/>
+      <c r="G119" s="25"/>
+      <c r="H119" s="25"/>
+      <c r="I119" s="26"/>
+      <c r="J119" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="K119" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="L119" s="48"/>
+      <c r="M119" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="120" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B120" s="26"/>
-      <c r="C120" s="26"/>
-      <c r="D120" s="26"/>
-      <c r="E120" s="26"/>
-      <c r="F120" s="26"/>
-      <c r="G120" s="26"/>
-      <c r="H120" s="26"/>
-      <c r="I120" s="27"/>
-      <c r="J120" s="34" t="s">
-        <v>282</v>
-      </c>
-      <c r="K120" s="35" t="s">
-        <v>283</v>
-      </c>
-      <c r="L120" s="40"/>
-      <c r="M120" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B120" s="25"/>
+      <c r="C120" s="25"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="25"/>
+      <c r="G120" s="25"/>
+      <c r="H120" s="25"/>
+      <c r="I120" s="26"/>
+      <c r="J120" s="33" t="s">
+        <v>275</v>
+      </c>
+      <c r="K120" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="L120" s="49"/>
+      <c r="M120" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" s="26"/>
-      <c r="C121" s="26"/>
-      <c r="D121" s="26"/>
-      <c r="E121" s="26"/>
-      <c r="F121" s="26"/>
-      <c r="G121" s="26"/>
-      <c r="H121" s="26"/>
-      <c r="I121" s="27"/>
-      <c r="J121" s="31" t="s">
-        <v>284</v>
-      </c>
-      <c r="K121" s="32" t="s">
-        <v>285</v>
-      </c>
-      <c r="L121" s="36" t="s">
-        <v>286</v>
-      </c>
-      <c r="M121" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B121" s="25"/>
+      <c r="C121" s="25"/>
+      <c r="D121" s="25"/>
+      <c r="E121" s="25"/>
+      <c r="F121" s="25"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="25"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="K121" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="L121" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="M121" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B122" s="26"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="26"/>
-      <c r="E122" s="26"/>
-      <c r="F122" s="26"/>
-      <c r="G122" s="26"/>
-      <c r="H122" s="26"/>
-      <c r="I122" s="27"/>
-      <c r="J122" s="33" t="s">
-        <v>287</v>
-      </c>
-      <c r="K122" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="L122" s="41"/>
-      <c r="M122" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B122" s="25"/>
+      <c r="C122" s="25"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="25"/>
+      <c r="G122" s="25"/>
+      <c r="H122" s="25"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="K122" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="L122" s="50"/>
+      <c r="M122" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="26"/>
-      <c r="E123" s="26"/>
-      <c r="F123" s="26"/>
-      <c r="G123" s="26"/>
-      <c r="H123" s="26"/>
-      <c r="I123" s="27"/>
-      <c r="J123" s="34" t="s">
-        <v>289</v>
-      </c>
-      <c r="K123" s="35" t="s">
-        <v>290</v>
-      </c>
-      <c r="L123" s="37"/>
-      <c r="M123" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B123" s="25"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="25"/>
+      <c r="E123" s="25"/>
+      <c r="F123" s="25"/>
+      <c r="G123" s="25"/>
+      <c r="H123" s="25"/>
+      <c r="I123" s="26"/>
+      <c r="J123" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="K123" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="L123" s="46"/>
+      <c r="M123" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="124" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B124" s="26"/>
-      <c r="C124" s="26"/>
-      <c r="D124" s="26"/>
-      <c r="E124" s="26"/>
-      <c r="F124" s="26"/>
-      <c r="G124" s="26"/>
-      <c r="H124" s="26"/>
-      <c r="I124" s="26"/>
-      <c r="J124" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="K124" s="54" t="s">
-        <v>292</v>
-      </c>
-      <c r="L124" s="30"/>
-      <c r="M124" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B124" s="25"/>
+      <c r="C124" s="25"/>
+      <c r="D124" s="25"/>
+      <c r="E124" s="25"/>
+      <c r="F124" s="25"/>
+      <c r="G124" s="25"/>
+      <c r="H124" s="25"/>
+      <c r="I124" s="25"/>
+      <c r="J124" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="K124" s="35" t="s">
+        <v>285</v>
+      </c>
+      <c r="L124" s="29"/>
+      <c r="M124" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="125" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B125" s="26"/>
-      <c r="C125" s="26"/>
-      <c r="D125" s="26"/>
-      <c r="E125" s="26"/>
-      <c r="F125" s="26"/>
-      <c r="G125" s="26"/>
-      <c r="H125" s="26"/>
-      <c r="I125" s="26"/>
-      <c r="J125" s="29" t="s">
-        <v>294</v>
-      </c>
-      <c r="K125" s="29" t="s">
-        <v>295</v>
-      </c>
-      <c r="L125" s="29"/>
-      <c r="M125" s="26" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B125" s="25"/>
+      <c r="C125" s="25"/>
+      <c r="D125" s="25"/>
+      <c r="E125" s="25"/>
+      <c r="F125" s="25"/>
+      <c r="G125" s="25"/>
+      <c r="H125" s="25"/>
+      <c r="I125" s="25"/>
+      <c r="J125" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="K125" s="28" t="s">
+        <v>288</v>
+      </c>
+      <c r="L125" s="28"/>
+      <c r="M125" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B126" s="26"/>
-      <c r="C126" s="26"/>
-      <c r="D126" s="26"/>
-      <c r="E126" s="26"/>
-      <c r="F126" s="26"/>
-      <c r="G126" s="26"/>
-      <c r="H126" s="26"/>
-      <c r="I126" s="27"/>
-      <c r="J126" s="31" t="s">
-        <v>296</v>
-      </c>
-      <c r="K126" s="32" t="s">
-        <v>297</v>
-      </c>
-      <c r="L126" s="36" t="s">
-        <v>300</v>
-      </c>
-      <c r="M126" s="28" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B126" s="25"/>
+      <c r="C126" s="25"/>
+      <c r="D126" s="25"/>
+      <c r="E126" s="25"/>
+      <c r="F126" s="25"/>
+      <c r="G126" s="25"/>
+      <c r="H126" s="25"/>
+      <c r="I126" s="26"/>
+      <c r="J126" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="K126" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="L126" s="45" t="s">
+        <v>293</v>
+      </c>
+      <c r="M126" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B127" s="26"/>
-      <c r="C127" s="26"/>
-      <c r="D127" s="26"/>
-      <c r="E127" s="26"/>
-      <c r="F127" s="26"/>
-      <c r="G127" s="26"/>
-      <c r="H127" s="26"/>
-      <c r="I127" s="27"/>
-      <c r="J127" s="34" t="s">
-        <v>298</v>
-      </c>
-      <c r="K127" s="35" t="s">
-        <v>299</v>
-      </c>
-      <c r="L127" s="37"/>
-      <c r="M127" s="53" t="s">
-        <v>88</v>
+        <v>23</v>
+      </c>
+      <c r="B127" s="25"/>
+      <c r="C127" s="25"/>
+      <c r="D127" s="25"/>
+      <c r="E127" s="25"/>
+      <c r="F127" s="25"/>
+      <c r="G127" s="25"/>
+      <c r="H127" s="25"/>
+      <c r="I127" s="26"/>
+      <c r="J127" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="K127" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="L127" s="46"/>
+      <c r="M127" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B128" s="26"/>
-      <c r="C128" s="26"/>
-      <c r="D128" s="26"/>
-      <c r="E128" s="26"/>
-      <c r="F128" s="26"/>
-      <c r="G128" s="26"/>
-      <c r="H128" s="26"/>
-      <c r="I128" s="26"/>
-      <c r="J128" s="30"/>
-      <c r="K128" s="30"/>
-      <c r="L128" s="30"/>
-      <c r="M128" s="26"/>
+        <v>23</v>
+      </c>
+      <c r="B128" s="25"/>
+      <c r="C128" s="25"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25"/>
+      <c r="F128" s="25"/>
+      <c r="G128" s="25"/>
+      <c r="H128" s="25"/>
+      <c r="I128" s="25"/>
+      <c r="J128" s="29"/>
+      <c r="K128" s="29"/>
+      <c r="L128" s="29"/>
+      <c r="M128" s="25"/>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B129" s="25"/>
+      <c r="C129" s="25"/>
+      <c r="D129" s="25" t="s">
+        <v>305</v>
+      </c>
+      <c r="E129" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="F129" s="25" t="s">
+        <v>307</v>
+      </c>
+      <c r="G129" s="25"/>
+      <c r="H129" s="25">
+        <v>26</v>
+      </c>
+      <c r="I129" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="J129" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="K129" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="L129" s="29"/>
+      <c r="M129" s="25"/>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A130" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B130" s="25"/>
+      <c r="C130" s="25"/>
+      <c r="D130" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="E130" s="25" t="s">
+        <v>304</v>
+      </c>
+      <c r="F130" s="25" t="s">
+        <v>308</v>
+      </c>
+      <c r="G130" s="25"/>
+      <c r="H130" s="25"/>
+      <c r="I130" s="25"/>
+      <c r="J130" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="K130" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="L130" s="29"/>
+      <c r="M130" s="25"/>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B131" s="25"/>
+      <c r="C131" s="25"/>
+      <c r="D131" s="25"/>
+      <c r="E131" s="25"/>
+      <c r="F131" s="25"/>
+      <c r="G131" s="25"/>
+      <c r="H131" s="25"/>
+      <c r="I131" s="25"/>
+      <c r="J131" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="K131" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="L131" s="29"/>
+      <c r="M131" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A132" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B132" s="25"/>
+      <c r="C132" s="25"/>
+      <c r="D132" s="25"/>
+      <c r="E132" s="25"/>
+      <c r="F132" s="25"/>
+      <c r="G132" s="25"/>
+      <c r="H132" s="25"/>
+      <c r="I132" s="25"/>
+      <c r="J132" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="K132" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="L132" s="29"/>
+      <c r="M132" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A133" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B133" s="25"/>
+      <c r="C133" s="25"/>
+      <c r="D133" s="25"/>
+      <c r="E133" s="25"/>
+      <c r="F133" s="25"/>
+      <c r="G133" s="25"/>
+      <c r="H133" s="25"/>
+      <c r="I133" s="25"/>
+      <c r="J133" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="K133" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="L133" s="29"/>
+      <c r="M133" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A134" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B134" s="25"/>
+      <c r="C134" s="25"/>
+      <c r="D134" s="25"/>
+      <c r="E134" s="25"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
+      <c r="H134" s="25"/>
+      <c r="I134" s="25"/>
+      <c r="J134" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="K134" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="L134" s="29"/>
+      <c r="M134" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A135" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B135" s="25"/>
+      <c r="C135" s="25"/>
+      <c r="D135" s="25"/>
+      <c r="E135" s="25"/>
+      <c r="F135" s="25"/>
+      <c r="G135" s="25"/>
+      <c r="H135" s="25"/>
+      <c r="I135" s="25"/>
+      <c r="J135" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="K135" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="L135" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="M135" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B136" s="36">
+        <v>1</v>
+      </c>
+      <c r="C136" s="25">
+        <v>0</v>
+      </c>
+      <c r="D136" s="25"/>
+      <c r="E136" s="25"/>
+      <c r="F136" s="25"/>
+      <c r="G136" s="25"/>
+      <c r="H136" s="25"/>
+      <c r="I136" s="25"/>
+      <c r="J136" s="37"/>
+      <c r="K136" s="37"/>
+      <c r="L136" s="43"/>
+      <c r="M136" s="25"/>
+    </row>
+    <row r="137" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B137" s="25"/>
+      <c r="C137" s="25"/>
+      <c r="D137" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="E137" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="F137" s="25"/>
+      <c r="G137" s="25"/>
+      <c r="H137" s="25"/>
+      <c r="I137" s="25"/>
+      <c r="J137" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="K137" s="40" t="s">
+        <v>325</v>
+      </c>
+      <c r="L137" s="43"/>
+      <c r="M137" s="25"/>
+    </row>
+    <row r="138" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B138" s="25"/>
+      <c r="C138" s="25"/>
+      <c r="D138" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="E138" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="F138" s="25"/>
+      <c r="G138" s="25"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="25"/>
+      <c r="J138" s="39"/>
+      <c r="K138" s="41"/>
+      <c r="L138" s="43"/>
+      <c r="M138" s="25"/>
+    </row>
+    <row r="139" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B139" s="25"/>
+      <c r="C139" s="25"/>
+      <c r="D139" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="E139" s="36">
+        <v>1</v>
+      </c>
+      <c r="F139" s="25"/>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="25"/>
+      <c r="J139" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="K139" s="29" t="s">
+        <v>328</v>
+      </c>
+      <c r="L139" s="43"/>
+      <c r="M139" s="25"/>
+    </row>
+    <row r="140" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B140" s="25"/>
+      <c r="C140" s="25"/>
+      <c r="D140" s="25"/>
+      <c r="E140" s="25"/>
+      <c r="F140" s="25"/>
+      <c r="G140" s="25"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="25"/>
+      <c r="J140" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="K140" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="L140" s="43"/>
+      <c r="M140" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B141" s="25"/>
+      <c r="C141" s="25"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="25"/>
+      <c r="G141" s="25"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="25"/>
+      <c r="J141" s="29" t="s">
+        <v>330</v>
+      </c>
+      <c r="K141" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="L141" s="43"/>
+      <c r="M141" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B142" s="25"/>
+      <c r="C142" s="25"/>
+      <c r="D142" s="25"/>
+      <c r="E142" s="25"/>
+      <c r="F142" s="25"/>
+      <c r="G142" s="25"/>
+      <c r="H142" s="25"/>
+      <c r="I142" s="25"/>
+      <c r="J142" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="K142" s="29" t="s">
+        <v>333</v>
+      </c>
+      <c r="L142" s="43"/>
+      <c r="M142" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B143" s="36"/>
+      <c r="C143" s="25"/>
+      <c r="D143" s="25"/>
+      <c r="E143" s="25"/>
+      <c r="F143" s="25"/>
+      <c r="G143" s="25"/>
+      <c r="H143" s="25"/>
+      <c r="I143" s="25"/>
+      <c r="J143" s="29" t="s">
+        <v>334</v>
+      </c>
+      <c r="K143" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="L143" s="43"/>
+      <c r="M143" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B144" s="25"/>
+      <c r="C144" s="25"/>
+      <c r="D144" s="25"/>
+      <c r="E144" s="36"/>
+      <c r="F144" s="25"/>
+      <c r="G144" s="25"/>
+      <c r="H144" s="25"/>
+      <c r="I144" s="25"/>
+      <c r="J144" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="K144" s="29" t="s">
+        <v>338</v>
+      </c>
+      <c r="L144" s="44"/>
+      <c r="M144" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A145" s="9"/>
+      <c r="B145" s="25"/>
+      <c r="C145" s="25"/>
+      <c r="D145" s="25"/>
+      <c r="E145" s="25"/>
+      <c r="F145" s="25"/>
+      <c r="G145" s="25"/>
+      <c r="H145" s="25"/>
+      <c r="I145" s="25"/>
+      <c r="J145" s="29"/>
+      <c r="K145" s="29"/>
+      <c r="L145" s="29"/>
+      <c r="M145" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="22">
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:M2"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="L28:L30"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="L34:L36"/>
+    <mergeCell ref="J137:J138"/>
+    <mergeCell ref="K137:K138"/>
+    <mergeCell ref="L135:L144"/>
+    <mergeCell ref="L102:L103"/>
+    <mergeCell ref="L80:L85"/>
+    <mergeCell ref="L94:L97"/>
+    <mergeCell ref="L98:L101"/>
     <mergeCell ref="L126:L127"/>
     <mergeCell ref="L104:L107"/>
     <mergeCell ref="L108:L111"/>
     <mergeCell ref="L113:L120"/>
     <mergeCell ref="L121:L123"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="L102:L103"/>
-    <mergeCell ref="L80:L85"/>
-    <mergeCell ref="L94:L97"/>
-    <mergeCell ref="L98:L101"/>
-    <mergeCell ref="J1:M2"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="L28:L30"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="L34:L36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4847,17 +5380,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated logic and bibliograpy and added some meson tests
</commit_message>
<xml_diff>
--- a/_docs/Logic.xlsx
+++ b/_docs/Logic.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="339">
   <si>
     <t>Name</t>
   </si>
@@ -1093,6 +1093,9 @@
   </si>
   <si>
     <t>Composite Types</t>
+  </si>
+  <si>
+    <t>ind type is defined in the nums module</t>
   </si>
 </sst>
 </file>
@@ -1569,39 +1572,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1640,6 +1610,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1942,13 +1945,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B127" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G149" sqref="G149"/>
+      <selection pane="bottomRight" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1969,47 +1972,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="46" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="48"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="43" t="s">
+      <c r="C2" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="40" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="50"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="63"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2465,7 +2468,7 @@
       <c r="J21" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="K21" s="51" t="s">
+      <c r="K21" s="40" t="s">
         <v>184</v>
       </c>
       <c r="L21" s="15" t="s">
@@ -2489,7 +2492,7 @@
       <c r="J22" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K22" s="52"/>
+      <c r="K22" s="41"/>
       <c r="L22" s="15" t="s">
         <v>66</v>
       </c>
@@ -2511,7 +2514,7 @@
       <c r="J23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="K23" s="52"/>
+      <c r="K23" s="41"/>
       <c r="L23" s="15" t="s">
         <v>66</v>
       </c>
@@ -2533,7 +2536,7 @@
       <c r="J24" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K24" s="52"/>
+      <c r="K24" s="41"/>
       <c r="L24" s="15" t="s">
         <v>66</v>
       </c>
@@ -2555,7 +2558,7 @@
       <c r="J25" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="K25" s="53"/>
+      <c r="K25" s="42"/>
       <c r="L25" s="15" t="s">
         <v>66</v>
       </c>
@@ -2621,7 +2624,7 @@
       <c r="J28" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="K28" s="51" t="s">
+      <c r="K28" s="40" t="s">
         <v>185</v>
       </c>
       <c r="L28" s="15" t="s">
@@ -2645,7 +2648,7 @@
       <c r="J29" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="K29" s="52"/>
+      <c r="K29" s="41"/>
       <c r="L29" s="15" t="s">
         <v>66</v>
       </c>
@@ -2667,7 +2670,7 @@
       <c r="J30" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="K30" s="52"/>
+      <c r="K30" s="41"/>
       <c r="L30" s="15" t="s">
         <v>66</v>
       </c>
@@ -2689,7 +2692,7 @@
       <c r="J31" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="K31" s="51" t="s">
+      <c r="K31" s="40" t="s">
         <v>186</v>
       </c>
       <c r="L31" s="15" t="s">
@@ -2713,7 +2716,7 @@
       <c r="J32" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="K32" s="52"/>
+      <c r="K32" s="41"/>
       <c r="L32" s="15" t="s">
         <v>66</v>
       </c>
@@ -2735,7 +2738,7 @@
       <c r="J33" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="K33" s="52"/>
+      <c r="K33" s="41"/>
       <c r="L33" s="15" t="s">
         <v>66</v>
       </c>
@@ -2757,7 +2760,7 @@
       <c r="J34" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="K34" s="51" t="s">
+      <c r="K34" s="40" t="s">
         <v>187</v>
       </c>
       <c r="L34" s="15" t="s">
@@ -2781,7 +2784,7 @@
       <c r="J35" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="K35" s="52"/>
+      <c r="K35" s="41"/>
       <c r="L35" s="15" t="s">
         <v>66</v>
       </c>
@@ -2803,7 +2806,7 @@
       <c r="J36" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="K36" s="53"/>
+      <c r="K36" s="42"/>
       <c r="L36" s="15" t="s">
         <v>66</v>
       </c>
@@ -3771,7 +3774,7 @@
       <c r="J80" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="K80" s="51" t="s">
+      <c r="K80" s="40" t="s">
         <v>201</v>
       </c>
       <c r="L80" s="15" t="s">
@@ -3795,7 +3798,7 @@
       <c r="J81" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="K81" s="52"/>
+      <c r="K81" s="41"/>
       <c r="L81" s="15" t="s">
         <v>66</v>
       </c>
@@ -3817,7 +3820,7 @@
       <c r="J82" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="K82" s="52"/>
+      <c r="K82" s="41"/>
       <c r="L82" s="15" t="s">
         <v>66</v>
       </c>
@@ -3839,7 +3842,7 @@
       <c r="J83" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="K83" s="52"/>
+      <c r="K83" s="41"/>
       <c r="L83" s="15" t="s">
         <v>66</v>
       </c>
@@ -3861,7 +3864,7 @@
       <c r="J84" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="K84" s="52"/>
+      <c r="K84" s="41"/>
       <c r="L84" s="15" t="s">
         <v>66</v>
       </c>
@@ -3883,7 +3886,7 @@
       <c r="J85" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="K85" s="53"/>
+      <c r="K85" s="42"/>
       <c r="L85" s="15" t="s">
         <v>66</v>
       </c>
@@ -4083,7 +4086,7 @@
       <c r="J94" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="K94" s="51" t="s">
+      <c r="K94" s="40" t="s">
         <v>224</v>
       </c>
       <c r="L94" s="27" t="s">
@@ -4107,7 +4110,7 @@
       <c r="J95" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="K95" s="52"/>
+      <c r="K95" s="41"/>
       <c r="L95" s="27" t="s">
         <v>66</v>
       </c>
@@ -4129,7 +4132,7 @@
       <c r="J96" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="K96" s="52"/>
+      <c r="K96" s="41"/>
       <c r="L96" s="27" t="s">
         <v>66</v>
       </c>
@@ -4151,7 +4154,7 @@
       <c r="J97" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="K97" s="53"/>
+      <c r="K97" s="42"/>
       <c r="L97" s="27" t="s">
         <v>66</v>
       </c>
@@ -4173,7 +4176,7 @@
       <c r="J98" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="K98" s="61" t="s">
+      <c r="K98" s="50" t="s">
         <v>233</v>
       </c>
       <c r="L98" s="27" t="s">
@@ -4197,7 +4200,7 @@
       <c r="J99" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="K99" s="63"/>
+      <c r="K99" s="52"/>
       <c r="L99" s="27" t="s">
         <v>66</v>
       </c>
@@ -4219,7 +4222,7 @@
       <c r="J100" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="K100" s="63"/>
+      <c r="K100" s="52"/>
       <c r="L100" s="27" t="s">
         <v>66</v>
       </c>
@@ -4241,7 +4244,7 @@
       <c r="J101" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="K101" s="62"/>
+      <c r="K101" s="51"/>
       <c r="L101" s="27" t="s">
         <v>66</v>
       </c>
@@ -4263,7 +4266,7 @@
       <c r="J102" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="K102" s="61" t="s">
+      <c r="K102" s="50" t="s">
         <v>238</v>
       </c>
       <c r="L102" s="27" t="s">
@@ -4287,7 +4290,7 @@
       <c r="J103" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="K103" s="62"/>
+      <c r="K103" s="51"/>
       <c r="L103" s="27" t="s">
         <v>66</v>
       </c>
@@ -4309,7 +4312,7 @@
       <c r="J104" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="K104" s="51" t="s">
+      <c r="K104" s="40" t="s">
         <v>247</v>
       </c>
       <c r="L104" s="27" t="s">
@@ -4333,7 +4336,7 @@
       <c r="J105" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="K105" s="52"/>
+      <c r="K105" s="41"/>
       <c r="L105" s="27" t="s">
         <v>66</v>
       </c>
@@ -4355,7 +4358,7 @@
       <c r="J106" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="K106" s="52"/>
+      <c r="K106" s="41"/>
       <c r="L106" s="27" t="s">
         <v>66</v>
       </c>
@@ -4377,7 +4380,7 @@
       <c r="J107" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="K107" s="53"/>
+      <c r="K107" s="42"/>
       <c r="L107" s="27" t="s">
         <v>66</v>
       </c>
@@ -4399,7 +4402,7 @@
       <c r="J108" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="K108" s="51" t="s">
+      <c r="K108" s="40" t="s">
         <v>256</v>
       </c>
       <c r="L108" s="27" t="s">
@@ -4423,7 +4426,7 @@
       <c r="J109" s="25" t="s">
         <v>251</v>
       </c>
-      <c r="K109" s="52"/>
+      <c r="K109" s="41"/>
       <c r="L109" s="27" t="s">
         <v>66</v>
       </c>
@@ -4445,7 +4448,7 @@
       <c r="J110" s="25" t="s">
         <v>253</v>
       </c>
-      <c r="K110" s="52"/>
+      <c r="K110" s="41"/>
       <c r="L110" s="27" t="s">
         <v>66</v>
       </c>
@@ -4467,7 +4470,7 @@
       <c r="J111" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="K111" s="53"/>
+      <c r="K111" s="42"/>
       <c r="L111" s="27" t="s">
         <v>66</v>
       </c>
@@ -4511,7 +4514,7 @@
       <c r="J113" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="K113" s="51" t="s">
+      <c r="K113" s="40" t="s">
         <v>269</v>
       </c>
       <c r="L113" s="27" t="s">
@@ -4535,7 +4538,7 @@
       <c r="J114" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="K114" s="52"/>
+      <c r="K114" s="41"/>
       <c r="L114" s="27" t="s">
         <v>66</v>
       </c>
@@ -4557,7 +4560,7 @@
       <c r="J115" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="K115" s="52"/>
+      <c r="K115" s="41"/>
       <c r="L115" s="27" t="s">
         <v>66</v>
       </c>
@@ -4579,7 +4582,7 @@
       <c r="J116" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="K116" s="52"/>
+      <c r="K116" s="41"/>
       <c r="L116" s="27" t="s">
         <v>66</v>
       </c>
@@ -4601,7 +4604,7 @@
       <c r="J117" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="K117" s="52"/>
+      <c r="K117" s="41"/>
       <c r="L117" s="27" t="s">
         <v>66</v>
       </c>
@@ -4623,7 +4626,7 @@
       <c r="J118" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="K118" s="52"/>
+      <c r="K118" s="41"/>
       <c r="L118" s="27" t="s">
         <v>66</v>
       </c>
@@ -4645,7 +4648,7 @@
       <c r="J119" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="K119" s="52"/>
+      <c r="K119" s="41"/>
       <c r="L119" s="27" t="s">
         <v>66</v>
       </c>
@@ -4667,7 +4670,7 @@
       <c r="J120" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="K120" s="53"/>
+      <c r="K120" s="42"/>
       <c r="L120" s="27" t="s">
         <v>66</v>
       </c>
@@ -4689,7 +4692,7 @@
       <c r="J121" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="K121" s="61" t="s">
+      <c r="K121" s="50" t="s">
         <v>276</v>
       </c>
       <c r="L121" s="27" t="s">
@@ -4713,7 +4716,7 @@
       <c r="J122" s="25" t="s">
         <v>278</v>
       </c>
-      <c r="K122" s="63"/>
+      <c r="K122" s="52"/>
       <c r="L122" s="27" t="s">
         <v>66</v>
       </c>
@@ -4735,7 +4738,7 @@
       <c r="J123" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="K123" s="62"/>
+      <c r="K123" s="51"/>
       <c r="L123" s="27" t="s">
         <v>66</v>
       </c>
@@ -4801,7 +4804,7 @@
       <c r="J126" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="K126" s="61" t="s">
+      <c r="K126" s="50" t="s">
         <v>290</v>
       </c>
       <c r="L126" s="27" t="s">
@@ -4825,7 +4828,7 @@
       <c r="J127" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="K127" s="62"/>
+      <c r="K127" s="51"/>
       <c r="L127" s="25" t="s">
         <v>66</v>
       </c>
@@ -5007,7 +5010,7 @@
       <c r="J135" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K135" s="58" t="s">
+      <c r="K135" s="47" t="s">
         <v>336</v>
       </c>
       <c r="L135" s="25" t="s">
@@ -5029,7 +5032,7 @@
       <c r="H136" s="25"/>
       <c r="I136" s="37"/>
       <c r="J136" s="37"/>
-      <c r="K136" s="59"/>
+      <c r="K136" s="48"/>
       <c r="L136" s="25"/>
     </row>
     <row r="137" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5047,13 +5050,13 @@
       <c r="F137" s="25"/>
       <c r="G137" s="25"/>
       <c r="H137" s="25"/>
-      <c r="I137" s="54" t="s">
+      <c r="I137" s="43" t="s">
         <v>321</v>
       </c>
-      <c r="J137" s="56" t="s">
+      <c r="J137" s="45" t="s">
         <v>322</v>
       </c>
-      <c r="K137" s="59"/>
+      <c r="K137" s="48"/>
       <c r="L137" s="25"/>
     </row>
     <row r="138" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5071,9 +5074,9 @@
       <c r="F138" s="25"/>
       <c r="G138" s="25"/>
       <c r="H138" s="25"/>
-      <c r="I138" s="55"/>
-      <c r="J138" s="57"/>
-      <c r="K138" s="59"/>
+      <c r="I138" s="44"/>
+      <c r="J138" s="46"/>
+      <c r="K138" s="48"/>
       <c r="L138" s="25"/>
     </row>
     <row r="139" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5097,7 +5100,7 @@
       <c r="J139" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="K139" s="59"/>
+      <c r="K139" s="48"/>
       <c r="L139" s="25"/>
     </row>
     <row r="140" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5117,7 +5120,7 @@
       <c r="J140" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="K140" s="59"/>
+      <c r="K140" s="48"/>
       <c r="L140" s="25" t="s">
         <v>66</v>
       </c>
@@ -5139,7 +5142,7 @@
       <c r="J141" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="K141" s="59"/>
+      <c r="K141" s="48"/>
       <c r="L141" s="25" t="s">
         <v>66</v>
       </c>
@@ -5161,7 +5164,7 @@
       <c r="J142" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="K142" s="59"/>
+      <c r="K142" s="48"/>
       <c r="L142" s="25" t="s">
         <v>66</v>
       </c>
@@ -5183,7 +5186,7 @@
       <c r="J143" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="K143" s="59"/>
+      <c r="K143" s="48"/>
       <c r="L143" s="25" t="s">
         <v>66</v>
       </c>
@@ -5205,7 +5208,7 @@
       <c r="J144" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="K144" s="60"/>
+      <c r="K144" s="49"/>
       <c r="L144" s="25" t="s">
         <v>66</v>
       </c>
@@ -5224,8 +5227,18 @@
       <c r="K145" s="29"/>
       <c r="L145" s="25"/>
     </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B148" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:L2"/>
     <mergeCell ref="K21:K25"/>
     <mergeCell ref="K28:K30"/>
     <mergeCell ref="K31:K33"/>
@@ -5242,11 +5255,6 @@
     <mergeCell ref="K108:K111"/>
     <mergeCell ref="K113:K120"/>
     <mergeCell ref="K121:K123"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>